<commit_message>
docs: Updating Requisitos.xlsx File
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS\Repos\Projeto Logistic\ProjetoLogistica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0C94FF1-C111-4062-B2FF-FF7F29F387C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498E9ACE-3A7A-4E78-85CB-4DE1806DCE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CD592D4B-4ADF-4CA0-9DA1-F296FD7CCAAD}"/>
   </bookViews>
@@ -527,7 +527,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,7 +594,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -628,7 +628,7 @@
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -645,7 +645,7 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -696,7 +696,7 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -713,7 +713,7 @@
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -764,7 +764,7 @@
         <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -781,7 +781,7 @@
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -832,7 +832,7 @@
         <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -849,7 +849,7 @@
         <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -883,7 +883,7 @@
         <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -897,7 +897,7 @@
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -911,7 +911,7 @@
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -953,7 +953,7 @@
         <v>32</v>
       </c>
       <c r="E26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -970,7 +970,7 @@
         <v>32</v>
       </c>
       <c r="E27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -998,7 +998,7 @@
         <v>8</v>
       </c>
       <c r="E29" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1012,7 +1012,7 @@
         <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>